<commit_message>
Highlighted the rows which need to remove
after discussion.
</commit_message>
<xml_diff>
--- a/Support/Configuration Management/MSTL_CMLIST.xlsx
+++ b/Support/Configuration Management/MSTL_CMLIST.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="3" r:id="rId1"/>
@@ -569,12 +569,18 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -610,7 +616,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -637,6 +643,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -1000,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2520,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2787,155 +2801,155 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="B15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="3" t="s">
+      <c r="B16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2977,41 +2991,41 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" s="3" t="s">
+      <c r="B18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3813,269 +3827,269 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B40" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" t="s">
-        <v>18</v>
-      </c>
-      <c r="H40" t="s">
-        <v>18</v>
-      </c>
-      <c r="I40" t="s">
-        <v>20</v>
-      </c>
-      <c r="J40" t="s">
-        <v>20</v>
-      </c>
-      <c r="K40" t="s">
-        <v>19</v>
-      </c>
-      <c r="L40" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="B40" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L40" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" t="s">
-        <v>19</v>
-      </c>
-      <c r="I41" t="s">
-        <v>20</v>
-      </c>
-      <c r="J41" t="s">
-        <v>20</v>
-      </c>
-      <c r="K41" t="s">
-        <v>19</v>
-      </c>
-      <c r="L41" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="B41" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I41" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K41" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" t="s">
-        <v>19</v>
-      </c>
-      <c r="E42" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" t="s">
-        <v>19</v>
-      </c>
-      <c r="H42" t="s">
-        <v>19</v>
-      </c>
-      <c r="I42" t="s">
-        <v>20</v>
-      </c>
-      <c r="J42" t="s">
-        <v>20</v>
-      </c>
-      <c r="K42" t="s">
-        <v>19</v>
-      </c>
-      <c r="L42" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="B42" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J42" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K42" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L42" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" t="s">
-        <v>19</v>
-      </c>
-      <c r="G43" t="s">
-        <v>19</v>
-      </c>
-      <c r="H43" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" t="s">
-        <v>19</v>
-      </c>
-      <c r="J43" t="s">
-        <v>19</v>
-      </c>
-      <c r="K43" t="s">
-        <v>19</v>
-      </c>
-      <c r="L43" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="B43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L43" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" t="s">
-        <v>19</v>
-      </c>
-      <c r="G44" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" t="s">
-        <v>18</v>
-      </c>
-      <c r="I44" t="s">
-        <v>19</v>
-      </c>
-      <c r="J44" t="s">
-        <v>19</v>
-      </c>
-      <c r="K44" t="s">
-        <v>19</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="B44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="B45" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" t="s">
-        <v>19</v>
-      </c>
-      <c r="H45" t="s">
-        <v>19</v>
-      </c>
-      <c r="I45" t="s">
-        <v>19</v>
-      </c>
-      <c r="J45" t="s">
-        <v>19</v>
-      </c>
-      <c r="K45" t="s">
-        <v>19</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="B45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L45" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B46" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" t="s">
-        <v>19</v>
-      </c>
-      <c r="E46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
-        <v>19</v>
-      </c>
-      <c r="G46" t="s">
-        <v>19</v>
-      </c>
-      <c r="H46" t="s">
-        <v>19</v>
-      </c>
-      <c r="I46" t="s">
-        <v>19</v>
-      </c>
-      <c r="J46" t="s">
-        <v>19</v>
-      </c>
-      <c r="K46" t="s">
-        <v>19</v>
-      </c>
-      <c r="L46" s="3" t="s">
+      <c r="B46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K46" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L46" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4459,41 +4473,41 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B57" t="s">
-        <v>18</v>
-      </c>
-      <c r="C57" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" t="s">
-        <v>18</v>
-      </c>
-      <c r="F57" t="s">
-        <v>18</v>
-      </c>
-      <c r="G57" t="s">
-        <v>18</v>
-      </c>
-      <c r="H57" t="s">
-        <v>18</v>
-      </c>
-      <c r="I57" t="s">
-        <v>18</v>
-      </c>
-      <c r="J57" t="s">
-        <v>18</v>
-      </c>
-      <c r="K57" t="s">
-        <v>18</v>
-      </c>
-      <c r="L57" t="s">
+      <c r="B57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K57" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L57" s="15" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5029,41 +5043,41 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="8" t="s">
+    <row r="72" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="B72" t="s">
-        <v>20</v>
-      </c>
-      <c r="C72" t="s">
-        <v>20</v>
-      </c>
-      <c r="D72" t="s">
-        <v>20</v>
-      </c>
-      <c r="E72" t="s">
-        <v>20</v>
-      </c>
-      <c r="F72" t="s">
-        <v>20</v>
-      </c>
-      <c r="G72" t="s">
-        <v>20</v>
-      </c>
-      <c r="H72" t="s">
-        <v>19</v>
-      </c>
-      <c r="I72" t="s">
-        <v>20</v>
-      </c>
-      <c r="J72" t="s">
-        <v>20</v>
-      </c>
-      <c r="K72" t="s">
-        <v>20</v>
-      </c>
-      <c r="L72" t="s">
+      <c r="B72" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G72" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H72" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I72" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J72" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K72" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L72" s="15" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5143,41 +5157,41 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
+    <row r="75" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B75" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G75" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H75" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I75" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J75" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K75" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L75" s="8" t="s">
+      <c r="B75" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G75" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H75" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I75" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J75" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K75" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="L75" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5232,18 +5246,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5296,14 +5310,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35FD17FA-4B4B-4751-8471-D81A3A4CBF4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41A3EE18-E916-4C0C-8547-FEF4A3A35D17}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -5313,6 +5319,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35FD17FA-4B4B-4751-8471-D81A3A4CBF4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>